<commit_message>
feat: Add two new specifications fields - operatingWeightRange and ratedPowerISO14396 - Database: Added operatingWeightRange (3.3) and ratedPowerISO14396 (7.7) to schema - Validators: Updated Zod schema to include both new fields - Excel Template: Added both fields (30 columns total now) - Frontend: Display new fields in details modal and machinery cards - Frontend: Include new fields in edit form data - All parts of the system now support these 30 specification fields
</commit_message>
<xml_diff>
--- a/backend-unified/public/templates/machinery-template.xlsx
+++ b/backend-unified/public/templates/machinery-template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,28 +408,30 @@
     <col min="4" max="4" width="30.83203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
     <col min="9" max="9" width="20.83203125" customWidth="1"/>
     <col min="10" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="11" width="22.83203125" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" customWidth="1"/>
     <col min="12" max="12" width="22.83203125" customWidth="1"/>
     <col min="13" max="13" width="22.83203125" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" customWidth="1"/>
+    <col min="14" max="14" width="22.83203125" customWidth="1"/>
     <col min="15" max="15" width="18.83203125" customWidth="1"/>
-    <col min="16" max="16" width="20.83203125" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" customWidth="1"/>
     <col min="17" max="17" width="20.83203125" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" customWidth="1"/>
-    <col min="19" max="19" width="18.83203125" customWidth="1"/>
-    <col min="20" max="20" width="25.83203125" customWidth="1"/>
-    <col min="21" max="21" width="25.83203125" customWidth="1"/>
-    <col min="22" max="22" width="18.83203125" customWidth="1"/>
+    <col min="18" max="18" width="25.83203125" customWidth="1"/>
+    <col min="19" max="19" width="20.83203125" customWidth="1"/>
+    <col min="20" max="20" width="18.83203125" customWidth="1"/>
+    <col min="21" max="21" width="18.83203125" customWidth="1"/>
+    <col min="22" max="22" width="25.83203125" customWidth="1"/>
     <col min="23" max="23" width="25.83203125" customWidth="1"/>
-    <col min="24" max="24" width="22.83203125" customWidth="1"/>
-    <col min="25" max="25" width="22.83203125" customWidth="1"/>
-    <col min="26" max="26" width="15.83203125" customWidth="1"/>
-    <col min="27" max="27" width="20.83203125" customWidth="1"/>
-    <col min="28" max="28" width="12.83203125" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" customWidth="1"/>
+    <col min="25" max="25" width="25.83203125" customWidth="1"/>
+    <col min="26" max="26" width="22.83203125" customWidth="1"/>
+    <col min="27" max="27" width="22.83203125" customWidth="1"/>
+    <col min="28" max="28" width="15.83203125" customWidth="1"/>
+    <col min="29" max="29" width="20.83203125" customWidth="1"/>
+    <col min="30" max="30" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -452,69 +454,75 @@
         <v>Cab Version Weight (kg)</v>
       </c>
       <c r="G1" t="str">
+        <v>Operating Weight Range (kg)</v>
+      </c>
+      <c r="H1" t="str">
         <v>Bucket Capacity (m³)</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>Emission Standard EU</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>Emission Standard EPA</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>Engine Model</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>Rated Power ISO9249 (kW)</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>Rated Power SAE J1349 (kW)</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>Rated Power EEC 80/1269 (kW)</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>Number of Cylinders</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>Bore x Stroke (mm)</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>Piston Displacement (L)</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
+        <v>Rated Power ISO14396 (kW)</v>
+      </c>
+      <c r="S1" t="str">
         <v>Implement Circuit (MPa)</v>
       </c>
-      <c r="R1" t="str">
+      <c r="T1" t="str">
         <v>Swing Circuit (MPa)</v>
       </c>
-      <c r="S1" t="str">
+      <c r="U1" t="str">
         <v>Travel Circuit (MPa)</v>
       </c>
-      <c r="T1" t="str">
+      <c r="V1" t="str">
         <v>Max Travel Speed High (km/h)</v>
       </c>
-      <c r="U1" t="str">
+      <c r="W1" t="str">
         <v>Max Travel Speed Low (km/h)</v>
       </c>
-      <c r="V1" t="str">
+      <c r="X1" t="str">
         <v>Swing Speed (min-1)</v>
       </c>
-      <c r="W1" t="str">
+      <c r="Y1" t="str">
         <v>Standard Track Shoe Width (mm)</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Z1" t="str">
         <v>Undercarriage Length (mm)</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="AA1" t="str">
         <v>Undercarriage Width (mm)</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AB1" t="str">
         <v>Fuel Tank (L)</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AC1" t="str">
         <v>Hydraulic System (L)</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AD1" t="str">
         <v>Availability</v>
       </c>
     </row>
@@ -538,19 +546,19 @@
         <v>3940</v>
       </c>
       <c r="G2">
+        <v>4000</v>
+      </c>
+      <c r="H2">
         <v>0.1</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>Stage III A</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>Interim Tier4</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <v>Yanmar EDM-3TNV88</v>
-      </c>
-      <c r="K2">
-        <v>21.2</v>
       </c>
       <c r="L2">
         <v>21.2</v>
@@ -559,54 +567,60 @@
         <v>21.2</v>
       </c>
       <c r="N2">
+        <v>21.2</v>
+      </c>
+      <c r="O2">
         <v>3</v>
       </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
         <v>88 x 90</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>1.642</v>
       </c>
-      <c r="Q2">
-        <v>24.5</v>
-      </c>
       <c r="R2">
-        <v>18.6</v>
+        <v>21.2</v>
       </c>
       <c r="S2">
         <v>24.5</v>
       </c>
       <c r="T2">
+        <v>18.6</v>
+      </c>
+      <c r="U2">
+        <v>24.5</v>
+      </c>
+      <c r="V2">
         <v>4.3</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>2.8</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>9.1</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>300</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>2110</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <v>1740</v>
       </c>
-      <c r="Z2">
+      <c r="AB2">
         <v>42</v>
       </c>
-      <c r="AA2">
+      <c r="AC2">
         <v>88</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AD2" t="str">
         <v>AVAILABLE</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AB2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AD2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Reorganize Excel template columns for logical order - Moved Operating Weight Range (kg) after Region Offerings - Moved Rated Power ISO14396 (kW) after Engine Model - Organized columns in logical groups: Basic Info, Region/Weight, Emissions, Engine/Power, Hydraulic, Undercarriage, Fuel/Capacity - Updated both frontend component and static template generator - Improved user experience with intuitive column order - Template now has 30 columns with professional organization
</commit_message>
<xml_diff>
--- a/backend-unified/public/templates/machinery-template.xlsx
+++ b/backend-unified/public/templates/machinery-template.xlsx
@@ -448,13 +448,13 @@
         <v>Region Offerings</v>
       </c>
       <c r="E1" t="str">
+        <v>Operating Weight Range (kg)</v>
+      </c>
+      <c r="F1" t="str">
         <v>Canopy Version Weight (kg)</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Cab Version Weight (kg)</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Operating Weight Range (kg)</v>
       </c>
       <c r="H1" t="str">
         <v>Bucket Capacity (m³)</v>
@@ -469,25 +469,25 @@
         <v>Engine Model</v>
       </c>
       <c r="L1" t="str">
+        <v>Rated Power ISO14396 (kW)</v>
+      </c>
+      <c r="M1" t="str">
         <v>Rated Power ISO9249 (kW)</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>Rated Power SAE J1349 (kW)</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>Rated Power EEC 80/1269 (kW)</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>Number of Cylinders</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>Bore x Stroke (mm)</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>Piston Displacement (L)</v>
-      </c>
-      <c r="R1" t="str">
-        <v>Rated Power ISO14396 (kW)</v>
       </c>
       <c r="S1" t="str">
         <v>Implement Circuit (MPa)</v>
@@ -540,13 +540,13 @@
         <v>SE Asia, Oceania, Europe</v>
       </c>
       <c r="E2">
+        <v>4000</v>
+      </c>
+      <c r="F2">
         <v>3770</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>3940</v>
-      </c>
-      <c r="G2">
-        <v>4000</v>
       </c>
       <c r="H2">
         <v>0.1</v>
@@ -570,16 +570,16 @@
         <v>21.2</v>
       </c>
       <c r="O2">
+        <v>21.2</v>
+      </c>
+      <c r="P2">
         <v>3</v>
       </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
         <v>88 x 90</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1.642</v>
-      </c>
-      <c r="R2">
-        <v>21.2</v>
       </c>
       <c r="S2">
         <v>24.5</v>

</xml_diff>